<commit_message>
US187994: mapping upload coded but not tested
</commit_message>
<xml_diff>
--- a/database/files/business-upload/mapping-upload.xlsx
+++ b/database/files/business-upload/mapping-upload.xlsx
@@ -19,12 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>User Note: Please begin populating this sheet with data from Row 6 leaving no space between data rows.</t>
   </si>
   <si>
     <t>User Note: Please populate values for all the columns that apply for that sub-measure. Incorrect or Blank fields will result in upload failure for that entire sub-measure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Sub Measure Name </t>
+  </si>
+  <si>
+    <t>Input Product value</t>
+  </si>
+  <si>
+    <t>Input Sales Value</t>
+  </si>
+  <si>
+    <t>Input Legal Entity Value</t>
+  </si>
+  <si>
+    <t>SCMS Segment</t>
+  </si>
+  <si>
+    <t>Input Business Entity Value</t>
   </si>
   <si>
     <r>
@@ -34,39 +52,13 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>indicates that the field is mandatory</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">*Sub Measure Name </t>
-  </si>
-  <si>
-    <t>Input Product value</t>
-  </si>
-  <si>
-    <t>Input Sales Value</t>
-  </si>
-  <si>
-    <t>Input Legal Entity Value</t>
-  </si>
-  <si>
-    <t>*Amount</t>
-  </si>
-  <si>
-    <t>SCMS Segment</t>
-  </si>
-  <si>
-    <t>Input Business Entity Value</t>
-  </si>
-  <si>
-    <t>Deal ID</t>
-  </si>
-  <si>
-    <t>Gross Unbilled Accrued Revenue Flag</t>
-  </si>
-  <si>
-    <t>Revenue Classification</t>
+    <t>*Percentage Value</t>
   </si>
 </sst>
 </file>
@@ -106,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +121,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -142,9 +143,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +455,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -463,85 +466,92 @@
     <col min="1" max="1" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="31.08984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="D4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>